<commit_message>
Improve run-time for PlantExp function.
</commit_message>
<xml_diff>
--- a/Data/Arabidopsis NLRs.xlsx
+++ b/Data/Arabidopsis NLRs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jexy2\OneDrive\Documents\PhD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42a5ee813758fc42/Documents/PhD/PhD.git/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DE7592-D2EB-42C3-B535-88D3D0E41D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -2864,8 +2864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191DFE7A-968B-4121-ADF6-CD647A0755EC}">
   <dimension ref="A1:K175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="78" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12561,15 +12561,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AAE124C5A4D68743B28650FDE78EA4DD" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2292b4748cb80aab9ce8557334a3a9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6db678f3-3207-45a7-bb76-4f6b54a03069" xmlns:ns4="f8cc16dc-7588-4949-9133-852c9419a450" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="532fccbb9916789b95418be1abc4b624" ns3:_="" ns4:_="">
     <xsd:import namespace="6db678f3-3207-45a7-bb76-4f6b54a03069"/>
@@ -12740,6 +12731,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8A9401F-48F2-48A8-9905-53282ECD946A}">
   <ds:schemaRefs>
@@ -12758,14 +12758,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A24C43BF-D402-4F87-99F4-C9E3E4401A98}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E07B35C2-85CE-44CD-8828-D423D51F09D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12784,6 +12776,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A24C43BF-D402-4F87-99F4-C9E3E4401A98}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{377e3d22-4ea1-422d-b0ad-8fcc89406b9e}" enabled="0" method="" siteId="{377e3d22-4ea1-422d-b0ad-8fcc89406b9e}" removed="1"/>

</xml_diff>

<commit_message>
Determine whether expression between genes within clusters is more similar than between all pairwise comparisons.
</commit_message>
<xml_diff>
--- a/Data/Arabidopsis NLRs.xlsx
+++ b/Data/Arabidopsis NLRs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42a5ee813758fc42/Documents/PhD/PhD.git/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{26DE7592-D2EB-42C3-B535-88D3D0E41D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF2749D4-ED06-4CFA-B41D-2EB9045FFA90}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="13_ncr:1_{26DE7592-D2EB-42C3-B535-88D3D0E41D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35D2BDAE-9099-4AAD-A3FD-9490603EB31E}"/>
   <bookViews>
-    <workbookView xWindow="16140" yWindow="1035" windowWidth="21600" windowHeight="11295" xr2:uid="{C4807C64-294B-40AB-88C6-14C535B56F75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C4807C64-294B-40AB-88C6-14C535B56F75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="788">
   <si>
     <t xml:space="preserve">Gene </t>
   </si>
@@ -2347,12 +2347,6 @@
     <t>single</t>
   </si>
   <si>
-    <t>cluster</t>
-  </si>
-  <si>
-    <t>double</t>
-  </si>
-  <si>
     <t>Minor cluster cAT5G47250</t>
   </si>
   <si>
@@ -2363,6 +2357,105 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>cluster 1</t>
+  </si>
+  <si>
+    <t>cluster 2</t>
+  </si>
+  <si>
+    <t>cluster 3</t>
+  </si>
+  <si>
+    <t>cluster 4</t>
+  </si>
+  <si>
+    <t>cluster 5</t>
+  </si>
+  <si>
+    <t>cluster 6</t>
+  </si>
+  <si>
+    <t>cluster 7</t>
+  </si>
+  <si>
+    <t>cluster 8</t>
+  </si>
+  <si>
+    <t>cluster 9</t>
+  </si>
+  <si>
+    <t>cluster 10</t>
+  </si>
+  <si>
+    <t>cluster 11</t>
+  </si>
+  <si>
+    <t>cluster 12</t>
+  </si>
+  <si>
+    <t>cluster 13</t>
+  </si>
+  <si>
+    <t>cluster 14</t>
+  </si>
+  <si>
+    <t>cluster 15</t>
+  </si>
+  <si>
+    <t>cluster 16</t>
+  </si>
+  <si>
+    <t>cluster 17</t>
+  </si>
+  <si>
+    <t>cluster 18</t>
+  </si>
+  <si>
+    <t>cluster 19</t>
+  </si>
+  <si>
+    <t>cluster 20</t>
+  </si>
+  <si>
+    <t>cluster 21</t>
+  </si>
+  <si>
+    <t>cluster 22</t>
+  </si>
+  <si>
+    <t>cluster 23</t>
+  </si>
+  <si>
+    <t>cluster 24</t>
+  </si>
+  <si>
+    <t>cluster 25</t>
+  </si>
+  <si>
+    <t>cluster 26</t>
+  </si>
+  <si>
+    <t>cluster 27</t>
+  </si>
+  <si>
+    <t>cluster 28</t>
+  </si>
+  <si>
+    <t>cluster 29</t>
+  </si>
+  <si>
+    <t>cluster 30</t>
+  </si>
+  <si>
+    <t>cluster 31</t>
+  </si>
+  <si>
+    <t>cluster 32</t>
+  </si>
+  <si>
+    <t>cluster 33</t>
   </si>
 </sst>
 </file>
@@ -2575,6 +2668,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2876,8 +2973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191DFE7A-968B-4121-ADF6-CD647A0755EC}">
   <dimension ref="A1:Q175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="81" workbookViewId="0">
-      <selection activeCell="A174" sqref="A174"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="81" workbookViewId="0">
+      <selection activeCell="K175" sqref="K175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2992,7 +3089,7 @@
         <v>68</v>
       </c>
       <c r="K3" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>4</v>
@@ -3030,7 +3127,7 @@
         <v>68</v>
       </c>
       <c r="K4" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>581</v>
@@ -3064,7 +3161,7 @@
         <v>68</v>
       </c>
       <c r="K5" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>4</v>
@@ -3098,7 +3195,7 @@
         <v>68</v>
       </c>
       <c r="K6" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>583</v>
@@ -3170,7 +3267,7 @@
         <v>69</v>
       </c>
       <c r="K8" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>13</v>
@@ -3201,7 +3298,7 @@
         <v>69</v>
       </c>
       <c r="K9" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>13</v>
@@ -3236,7 +3333,7 @@
         <v>69</v>
       </c>
       <c r="K10" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>13</v>
@@ -3274,7 +3371,7 @@
         <v>69</v>
       </c>
       <c r="K11" t="s">
-        <v>752</v>
+        <v>757</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>587</v>
@@ -3312,7 +3409,7 @@
         <v>69</v>
       </c>
       <c r="K12" t="s">
-        <v>752</v>
+        <v>757</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>54</v>
@@ -3552,7 +3649,7 @@
         <v>69</v>
       </c>
       <c r="K19" t="s">
-        <v>751</v>
+        <v>758</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>28</v>
@@ -3590,7 +3687,7 @@
         <v>69</v>
       </c>
       <c r="K20" t="s">
-        <v>751</v>
+        <v>758</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>29</v>
@@ -3628,7 +3725,7 @@
         <v>69</v>
       </c>
       <c r="K21" t="s">
-        <v>751</v>
+        <v>758</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>594</v>
@@ -3695,7 +3792,7 @@
         <v>68</v>
       </c>
       <c r="K23" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>40</v>
@@ -3733,7 +3830,7 @@
         <v>68</v>
       </c>
       <c r="K24" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>595</v>
@@ -3771,7 +3868,7 @@
         <v>68</v>
       </c>
       <c r="K25" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>40</v>
@@ -3809,7 +3906,7 @@
         <v>68</v>
       </c>
       <c r="K26" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>39</v>
@@ -3844,7 +3941,7 @@
         <v>68</v>
       </c>
       <c r="K27" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>40</v>
@@ -3879,7 +3976,7 @@
         <v>68</v>
       </c>
       <c r="K28" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>40</v>
@@ -3914,7 +4011,7 @@
         <v>68</v>
       </c>
       <c r="K29" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>40</v>
@@ -3949,7 +4046,7 @@
         <v>68</v>
       </c>
       <c r="K30" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>40</v>
@@ -4057,7 +4154,7 @@
         <v>68</v>
       </c>
       <c r="K33" t="s">
-        <v>751</v>
+        <v>760</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>50</v>
@@ -4095,7 +4192,7 @@
         <v>68</v>
       </c>
       <c r="K34" t="s">
-        <v>751</v>
+        <v>760</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>48</v>
@@ -4133,7 +4230,7 @@
         <v>68</v>
       </c>
       <c r="K35" t="s">
-        <v>751</v>
+        <v>760</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>603</v>
@@ -4171,7 +4268,7 @@
         <v>68</v>
       </c>
       <c r="K36" t="s">
-        <v>751</v>
+        <v>760</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>49</v>
@@ -4240,7 +4337,7 @@
         <v>68</v>
       </c>
       <c r="K38" t="s">
-        <v>752</v>
+        <v>761</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>607</v>
@@ -4278,7 +4375,7 @@
         <v>68</v>
       </c>
       <c r="K39" t="s">
-        <v>752</v>
+        <v>761</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>609</v>
@@ -4316,7 +4413,7 @@
         <v>69</v>
       </c>
       <c r="K40" t="s">
-        <v>751</v>
+        <v>762</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>62</v>
@@ -4354,7 +4451,7 @@
         <v>69</v>
       </c>
       <c r="K41" t="s">
-        <v>751</v>
+        <v>762</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>611</v>
@@ -4392,7 +4489,7 @@
         <v>69</v>
       </c>
       <c r="K42" t="s">
-        <v>751</v>
+        <v>762</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>612</v>
@@ -4430,7 +4527,7 @@
         <v>69</v>
       </c>
       <c r="K43" t="s">
-        <v>751</v>
+        <v>762</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>613</v>
@@ -4465,7 +4562,7 @@
         <v>69</v>
       </c>
       <c r="K44" t="s">
-        <v>751</v>
+        <v>762</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>62</v>
@@ -4503,7 +4600,7 @@
         <v>69</v>
       </c>
       <c r="K45" t="s">
-        <v>751</v>
+        <v>762</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>62</v>
@@ -4538,7 +4635,7 @@
         <v>69</v>
       </c>
       <c r="K46" t="s">
-        <v>751</v>
+        <v>762</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>63</v>
@@ -4684,7 +4781,7 @@
         <v>69</v>
       </c>
       <c r="K50" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>83</v>
@@ -4715,7 +4812,7 @@
         <v>69</v>
       </c>
       <c r="K51" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>84</v>
@@ -4743,7 +4840,7 @@
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
       <c r="K52" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>82</v>
@@ -4770,7 +4867,7 @@
         <v>69</v>
       </c>
       <c r="K53" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>85</v>
@@ -4801,7 +4898,7 @@
         <v>69</v>
       </c>
       <c r="K54" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>86</v>
@@ -4839,7 +4936,7 @@
         <v>69</v>
       </c>
       <c r="K55" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>619</v>
@@ -4877,7 +4974,7 @@
         <v>69</v>
       </c>
       <c r="K56" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>621</v>
@@ -4915,7 +5012,7 @@
         <v>69</v>
       </c>
       <c r="K57" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>623</v>
@@ -4953,7 +5050,7 @@
         <v>69</v>
       </c>
       <c r="K58" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>87</v>
@@ -4991,7 +5088,7 @@
         <v>69</v>
       </c>
       <c r="K59" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>628</v>
@@ -5029,7 +5126,7 @@
         <v>69</v>
       </c>
       <c r="K60" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>629</v>
@@ -5060,7 +5157,7 @@
         <v>69</v>
       </c>
       <c r="K61" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="L61" s="1" t="s">
         <v>88</v>
@@ -5167,7 +5264,7 @@
         <v>69</v>
       </c>
       <c r="K64" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>95</v>
@@ -5202,7 +5299,7 @@
         <v>69</v>
       </c>
       <c r="K65" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>95</v>
@@ -5240,7 +5337,7 @@
         <v>69</v>
       </c>
       <c r="K66" t="s">
-        <v>752</v>
+        <v>765</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>632</v>
@@ -5278,7 +5375,7 @@
         <v>69</v>
       </c>
       <c r="K67" t="s">
-        <v>752</v>
+        <v>765</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>633</v>
@@ -5344,7 +5441,7 @@
         <v>673</v>
       </c>
       <c r="K69" t="s">
-        <v>752</v>
+        <v>766</v>
       </c>
       <c r="L69" s="1" t="s">
         <v>99</v>
@@ -5382,7 +5479,7 @@
         <v>68</v>
       </c>
       <c r="K70" t="s">
-        <v>752</v>
+        <v>766</v>
       </c>
       <c r="L70" s="1" t="s">
         <v>635</v>
@@ -5490,7 +5587,7 @@
         <v>69</v>
       </c>
       <c r="K73" t="s">
-        <v>751</v>
+        <v>767</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>106</v>
@@ -5524,7 +5621,7 @@
         <v>69</v>
       </c>
       <c r="K74" t="s">
-        <v>751</v>
+        <v>767</v>
       </c>
       <c r="L74" s="1" t="s">
         <v>107</v>
@@ -5562,7 +5659,7 @@
         <v>69</v>
       </c>
       <c r="K75" t="s">
-        <v>751</v>
+        <v>767</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>106</v>
@@ -5596,7 +5693,7 @@
         <v>69</v>
       </c>
       <c r="K76" t="s">
-        <v>751</v>
+        <v>767</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>108</v>
@@ -5630,7 +5727,7 @@
         <v>68</v>
       </c>
       <c r="K77" t="s">
-        <v>751</v>
+        <v>768</v>
       </c>
       <c r="L77" s="1" t="s">
         <v>113</v>
@@ -5665,7 +5762,7 @@
         <v>68</v>
       </c>
       <c r="K78" t="s">
-        <v>751</v>
+        <v>768</v>
       </c>
       <c r="L78" s="1" t="s">
         <v>112</v>
@@ -5696,7 +5793,7 @@
         <v>68</v>
       </c>
       <c r="K79" t="s">
-        <v>751</v>
+        <v>768</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>112</v>
@@ -5765,7 +5862,7 @@
         <v>69</v>
       </c>
       <c r="K81" t="s">
-        <v>752</v>
+        <v>769</v>
       </c>
       <c r="L81" s="1" t="s">
         <v>118</v>
@@ -5800,7 +5897,7 @@
         <v>69</v>
       </c>
       <c r="K82" t="s">
-        <v>752</v>
+        <v>769</v>
       </c>
       <c r="L82" s="1" t="s">
         <v>118</v>
@@ -5867,7 +5964,7 @@
         <v>69</v>
       </c>
       <c r="K84" t="s">
-        <v>751</v>
+        <v>770</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>123</v>
@@ -5905,7 +6002,7 @@
         <v>69</v>
       </c>
       <c r="K85" t="s">
-        <v>751</v>
+        <v>770</v>
       </c>
       <c r="L85" s="1" t="s">
         <v>748</v>
@@ -5936,7 +6033,7 @@
         <v>69</v>
       </c>
       <c r="K86" t="s">
-        <v>751</v>
+        <v>770</v>
       </c>
       <c r="L86" s="1" t="s">
         <v>123</v>
@@ -6036,7 +6133,7 @@
         <v>69</v>
       </c>
       <c r="K89" t="s">
-        <v>752</v>
+        <v>771</v>
       </c>
       <c r="L89" s="1" t="s">
         <v>643</v>
@@ -6070,7 +6167,7 @@
         <v>69</v>
       </c>
       <c r="K90" t="s">
-        <v>752</v>
+        <v>771</v>
       </c>
       <c r="L90" s="1" t="s">
         <v>130</v>
@@ -6146,7 +6243,7 @@
         <v>69</v>
       </c>
       <c r="K92" t="s">
-        <v>751</v>
+        <v>772</v>
       </c>
       <c r="L92" s="1" t="s">
         <v>646</v>
@@ -6184,7 +6281,7 @@
         <v>69</v>
       </c>
       <c r="K93" t="s">
-        <v>751</v>
+        <v>772</v>
       </c>
       <c r="L93" s="1" t="s">
         <v>647</v>
@@ -6222,7 +6319,7 @@
         <v>69</v>
       </c>
       <c r="K94" t="s">
-        <v>751</v>
+        <v>772</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>141</v>
@@ -6252,7 +6349,7 @@
         <v>69</v>
       </c>
       <c r="K95" t="s">
-        <v>751</v>
+        <v>772</v>
       </c>
       <c r="L95" s="1" t="s">
         <v>651</v>
@@ -6287,7 +6384,7 @@
         <v>69</v>
       </c>
       <c r="K96" t="s">
-        <v>751</v>
+        <v>772</v>
       </c>
       <c r="L96" s="1" t="s">
         <v>141</v>
@@ -6322,7 +6419,7 @@
         <v>69</v>
       </c>
       <c r="K97" t="s">
-        <v>751</v>
+        <v>772</v>
       </c>
       <c r="L97" s="1" t="s">
         <v>141</v>
@@ -6356,7 +6453,7 @@
         <v>69</v>
       </c>
       <c r="K98" t="s">
-        <v>751</v>
+        <v>772</v>
       </c>
       <c r="L98" s="1" t="s">
         <v>653</v>
@@ -6390,7 +6487,7 @@
         <v>69</v>
       </c>
       <c r="K99" t="s">
-        <v>751</v>
+        <v>772</v>
       </c>
       <c r="L99" s="1" t="s">
         <v>649</v>
@@ -6428,7 +6525,7 @@
         <v>69</v>
       </c>
       <c r="K100" t="s">
-        <v>751</v>
+        <v>772</v>
       </c>
       <c r="L100" s="1" t="s">
         <v>142</v>
@@ -6466,7 +6563,7 @@
         <v>69</v>
       </c>
       <c r="K101" t="s">
-        <v>751</v>
+        <v>773</v>
       </c>
       <c r="L101" s="1" t="s">
         <v>148</v>
@@ -6504,7 +6601,7 @@
         <v>69</v>
       </c>
       <c r="K102" t="s">
-        <v>751</v>
+        <v>773</v>
       </c>
       <c r="L102" s="1" t="s">
         <v>148</v>
@@ -6542,7 +6639,7 @@
         <v>69</v>
       </c>
       <c r="K103" t="s">
-        <v>751</v>
+        <v>773</v>
       </c>
       <c r="L103" s="1" t="s">
         <v>147</v>
@@ -6580,7 +6677,7 @@
         <v>69</v>
       </c>
       <c r="K104" t="s">
-        <v>751</v>
+        <v>773</v>
       </c>
       <c r="L104" s="1" t="s">
         <v>148</v>
@@ -6698,7 +6795,7 @@
         <v>68</v>
       </c>
       <c r="K108" t="s">
-        <v>752</v>
+        <v>774</v>
       </c>
       <c r="L108" s="1" t="s">
         <v>154</v>
@@ -6733,7 +6830,7 @@
         <v>68</v>
       </c>
       <c r="K109" t="s">
-        <v>752</v>
+        <v>774</v>
       </c>
       <c r="L109" s="1" t="s">
         <v>154</v>
@@ -6793,7 +6890,7 @@
         <v>69</v>
       </c>
       <c r="K111" t="s">
-        <v>752</v>
+        <v>775</v>
       </c>
       <c r="L111" s="1" t="s">
         <v>159</v>
@@ -6827,7 +6924,7 @@
         <v>69</v>
       </c>
       <c r="K112" t="s">
-        <v>752</v>
+        <v>775</v>
       </c>
       <c r="L112" s="1" t="s">
         <v>666</v>
@@ -7007,7 +7104,7 @@
         <v>69</v>
       </c>
       <c r="K117" t="s">
-        <v>751</v>
+        <v>776</v>
       </c>
       <c r="L117" s="1" t="s">
         <v>169</v>
@@ -7045,7 +7142,7 @@
         <v>69</v>
       </c>
       <c r="K118" t="s">
-        <v>751</v>
+        <v>776</v>
       </c>
       <c r="L118" s="1" t="s">
         <v>168</v>
@@ -7080,7 +7177,7 @@
         <v>69</v>
       </c>
       <c r="K119" t="s">
-        <v>751</v>
+        <v>776</v>
       </c>
       <c r="L119" s="1" t="s">
         <v>170</v>
@@ -7115,7 +7212,7 @@
         <v>69</v>
       </c>
       <c r="K120" t="s">
-        <v>751</v>
+        <v>777</v>
       </c>
       <c r="L120" s="1" t="s">
         <v>174</v>
@@ -7153,7 +7250,7 @@
         <v>69</v>
       </c>
       <c r="K121" t="s">
-        <v>751</v>
+        <v>777</v>
       </c>
       <c r="L121" s="1" t="s">
         <v>175</v>
@@ -7191,7 +7288,7 @@
         <v>69</v>
       </c>
       <c r="K122" t="s">
-        <v>751</v>
+        <v>777</v>
       </c>
       <c r="L122" s="1" t="s">
         <v>176</v>
@@ -7508,7 +7605,7 @@
         <v>69</v>
       </c>
       <c r="K131" t="s">
-        <v>752</v>
+        <v>778</v>
       </c>
       <c r="L131" s="1" t="s">
         <v>189</v>
@@ -7542,7 +7639,7 @@
         <v>69</v>
       </c>
       <c r="K132" t="s">
-        <v>752</v>
+        <v>778</v>
       </c>
       <c r="L132" s="1" t="s">
         <v>188</v>
@@ -7580,7 +7677,7 @@
         <v>69</v>
       </c>
       <c r="K133" t="s">
-        <v>751</v>
+        <v>779</v>
       </c>
       <c r="L133" s="1" t="s">
         <v>196</v>
@@ -7615,7 +7712,7 @@
         <v>69</v>
       </c>
       <c r="K134" t="s">
-        <v>751</v>
+        <v>779</v>
       </c>
       <c r="L134" s="1" t="s">
         <v>196</v>
@@ -7653,7 +7750,7 @@
         <v>69</v>
       </c>
       <c r="K135" t="s">
-        <v>751</v>
+        <v>779</v>
       </c>
       <c r="L135" s="1" t="s">
         <v>686</v>
@@ -7691,7 +7788,7 @@
         <v>69</v>
       </c>
       <c r="K136" t="s">
-        <v>751</v>
+        <v>779</v>
       </c>
       <c r="L136" s="1" t="s">
         <v>195</v>
@@ -7729,7 +7826,7 @@
         <v>69</v>
       </c>
       <c r="K137" t="s">
-        <v>751</v>
+        <v>779</v>
       </c>
       <c r="L137" s="1" t="s">
         <v>694</v>
@@ -7794,7 +7891,7 @@
         <v>68</v>
       </c>
       <c r="K139" t="s">
-        <v>751</v>
+        <v>780</v>
       </c>
       <c r="L139" s="1" t="s">
         <v>202</v>
@@ -7828,7 +7925,7 @@
         <v>68</v>
       </c>
       <c r="K140" t="s">
-        <v>751</v>
+        <v>780</v>
       </c>
       <c r="L140" s="1" t="s">
         <v>202</v>
@@ -7862,7 +7959,7 @@
         <v>68</v>
       </c>
       <c r="K141" t="s">
-        <v>751</v>
+        <v>780</v>
       </c>
       <c r="L141" s="1" t="s">
         <v>698</v>
@@ -7934,7 +8031,7 @@
         <v>69</v>
       </c>
       <c r="K143" t="s">
-        <v>751</v>
+        <v>781</v>
       </c>
       <c r="L143" s="1" t="s">
         <v>600</v>
@@ -7968,7 +8065,7 @@
         <v>69</v>
       </c>
       <c r="K144" t="s">
-        <v>751</v>
+        <v>781</v>
       </c>
       <c r="L144" s="1" t="s">
         <v>705</v>
@@ -8006,7 +8103,7 @@
         <v>69</v>
       </c>
       <c r="K145" t="s">
-        <v>751</v>
+        <v>781</v>
       </c>
       <c r="L145" s="1" t="s">
         <v>208</v>
@@ -8044,7 +8141,7 @@
         <v>69</v>
       </c>
       <c r="K146" t="s">
-        <v>751</v>
+        <v>781</v>
       </c>
       <c r="L146" s="1" t="s">
         <v>209</v>
@@ -8079,7 +8176,7 @@
         <v>69</v>
       </c>
       <c r="K147" t="s">
-        <v>751</v>
+        <v>782</v>
       </c>
       <c r="L147" s="1" t="s">
         <v>217</v>
@@ -8117,7 +8214,7 @@
         <v>69</v>
       </c>
       <c r="K148" t="s">
-        <v>751</v>
+        <v>782</v>
       </c>
       <c r="L148" s="1" t="s">
         <v>217</v>
@@ -8152,7 +8249,7 @@
         <v>69</v>
       </c>
       <c r="K149" t="s">
-        <v>751</v>
+        <v>782</v>
       </c>
       <c r="L149" s="1" t="s">
         <v>217</v>
@@ -8187,7 +8284,7 @@
         <v>69</v>
       </c>
       <c r="K150" t="s">
-        <v>751</v>
+        <v>782</v>
       </c>
       <c r="L150" s="1" t="s">
         <v>217</v>
@@ -8222,7 +8319,7 @@
         <v>69</v>
       </c>
       <c r="K151" t="s">
-        <v>751</v>
+        <v>782</v>
       </c>
       <c r="L151" s="1" t="s">
         <v>217</v>
@@ -8260,7 +8357,7 @@
         <v>69</v>
       </c>
       <c r="K152" t="s">
-        <v>751</v>
+        <v>782</v>
       </c>
       <c r="L152" s="1" t="s">
         <v>218</v>
@@ -8298,7 +8395,7 @@
         <v>69</v>
       </c>
       <c r="K153" t="s">
-        <v>751</v>
+        <v>782</v>
       </c>
       <c r="L153" s="1" t="s">
         <v>217</v>
@@ -8333,7 +8430,7 @@
         <v>163</v>
       </c>
       <c r="K154" t="s">
-        <v>752</v>
+        <v>783</v>
       </c>
       <c r="L154" s="1" t="s">
         <v>221</v>
@@ -8362,7 +8459,7 @@
       </c>
       <c r="I155" s="16"/>
       <c r="K155" t="s">
-        <v>752</v>
+        <v>783</v>
       </c>
       <c r="L155" s="1" t="s">
         <v>221</v>
@@ -8400,7 +8497,7 @@
         <v>69</v>
       </c>
       <c r="K156" t="s">
-        <v>751</v>
+        <v>784</v>
       </c>
       <c r="L156" s="1" t="s">
         <v>229</v>
@@ -8438,7 +8535,7 @@
         <v>69</v>
       </c>
       <c r="K157" t="s">
-        <v>751</v>
+        <v>784</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>715</v>
@@ -8476,7 +8573,7 @@
         <v>69</v>
       </c>
       <c r="K158" t="s">
-        <v>751</v>
+        <v>784</v>
       </c>
       <c r="L158" s="1" t="s">
         <v>229</v>
@@ -8514,7 +8611,7 @@
         <v>69</v>
       </c>
       <c r="K159" t="s">
-        <v>751</v>
+        <v>784</v>
       </c>
       <c r="L159" s="1" t="s">
         <v>230</v>
@@ -8552,7 +8649,7 @@
         <v>69</v>
       </c>
       <c r="K160" t="s">
-        <v>751</v>
+        <v>784</v>
       </c>
       <c r="L160" s="1" t="s">
         <v>229</v>
@@ -8590,7 +8687,7 @@
         <v>69</v>
       </c>
       <c r="K161" t="s">
-        <v>751</v>
+        <v>784</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>229</v>
@@ -8628,7 +8725,7 @@
         <v>69</v>
       </c>
       <c r="K162" t="s">
-        <v>751</v>
+        <v>784</v>
       </c>
       <c r="L162" s="1" t="s">
         <v>727</v>
@@ -8663,7 +8760,7 @@
         <v>68</v>
       </c>
       <c r="K163" t="s">
-        <v>751</v>
+        <v>785</v>
       </c>
       <c r="L163" s="1" t="s">
         <v>710</v>
@@ -8698,10 +8795,10 @@
         <v>68</v>
       </c>
       <c r="K164" t="s">
+        <v>785</v>
+      </c>
+      <c r="L164" s="1" t="s">
         <v>751</v>
-      </c>
-      <c r="L164" s="1" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.25">
@@ -8730,10 +8827,10 @@
         <v>19197039</v>
       </c>
       <c r="K165" t="s">
-        <v>751</v>
+        <v>785</v>
       </c>
       <c r="L165" s="1" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.25">
@@ -8795,7 +8892,7 @@
         <v>69</v>
       </c>
       <c r="K167" t="s">
-        <v>751</v>
+        <v>786</v>
       </c>
       <c r="L167" s="1" t="s">
         <v>239</v>
@@ -8823,7 +8920,7 @@
       <c r="G168" s="12"/>
       <c r="H168" s="12"/>
       <c r="K168" t="s">
-        <v>751</v>
+        <v>786</v>
       </c>
       <c r="L168" s="1" t="s">
         <v>239</v>
@@ -8858,10 +8955,10 @@
         <v>69</v>
       </c>
       <c r="K169" t="s">
-        <v>751</v>
+        <v>786</v>
       </c>
       <c r="L169" s="1" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.25">
@@ -8961,7 +9058,7 @@
         <v>247</v>
       </c>
       <c r="Q172" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.25">
@@ -9030,7 +9127,7 @@
         <v>240</v>
       </c>
       <c r="K174" t="s">
-        <v>752</v>
+        <v>787</v>
       </c>
       <c r="L174" s="1" t="s">
         <v>249</v>
@@ -9068,7 +9165,7 @@
         <v>240</v>
       </c>
       <c r="K175" t="s">
-        <v>752</v>
+        <v>787</v>
       </c>
       <c r="L175" s="1" t="s">
         <v>745</v>
@@ -13105,6 +13202,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AAE124C5A4D68743B28650FDE78EA4DD" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2292b4748cb80aab9ce8557334a3a9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6db678f3-3207-45a7-bb76-4f6b54a03069" xmlns:ns4="f8cc16dc-7588-4949-9133-852c9419a450" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="532fccbb9916789b95418be1abc4b624" ns3:_="" ns4:_="">
     <xsd:import namespace="6db678f3-3207-45a7-bb76-4f6b54a03069"/>
@@ -13275,12 +13378,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A24C43BF-D402-4F87-99F4-C9E3E4401A98}">
   <ds:schemaRefs>
@@ -13290,6 +13387,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8A9401F-48F2-48A8-9905-53282ECD946A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f8cc16dc-7588-4949-9133-852c9419a450"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="6db678f3-3207-45a7-bb76-4f6b54a03069"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E07B35C2-85CE-44CD-8828-D423D51F09D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13308,23 +13422,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8A9401F-48F2-48A8-9905-53282ECD946A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f8cc16dc-7588-4949-9133-852c9419a450"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="6db678f3-3207-45a7-bb76-4f6b54a03069"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{377e3d22-4ea1-422d-b0ad-8fcc89406b9e}" enabled="0" method="" siteId="{377e3d22-4ea1-422d-b0ad-8fcc89406b9e}" removed="1"/>

</xml_diff>